<commit_message>
added batch definitions to lemhi_winter_telemetry_tag_info.xlsx
</commit_message>
<xml_diff>
--- a/data/prepped/tag_release/lemhi_winter_telemetry_tag_info.xlsx
+++ b/data/prepped/tag_release/lemhi_winter_telemetry_tag_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikea\Desktop\tag_release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\telemetyr\data\prepped\tag_release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2987310F-0502-424E-8B9A-7A6B964FD985}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B42266-37DA-41C8-A715-AEF68E968ACC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="release_info" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7095" uniqueCount="1549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7107" uniqueCount="1556">
   <si>
     <t>season</t>
   </si>
@@ -4679,6 +4679,27 @@
   </si>
   <si>
     <t>Lost to river during read range testing</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>operate continuously upon operation (no shutdown)</t>
+  </si>
+  <si>
+    <t>operate for 1 day (24 hrs) upon activation, shutdown, and then re-activate at day 50</t>
+  </si>
+  <si>
+    <t>operate for 1 day (24 hrs) upon activation, shutdown, and then re-activate at day 100</t>
+  </si>
+  <si>
+    <t>sentinel</t>
+  </si>
+  <si>
+    <t>a pulse rate of 18 pulses per 15 minutes</t>
+  </si>
+  <si>
+    <t>operate for 1 hr upon activation, restart 48 hrs after activation, then operate for 1-week on and 1-week off for remaining life span</t>
   </si>
 </sst>
 </file>
@@ -5087,8 +5108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M777"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
@@ -36052,12 +36073,66 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849A2B6F-9B4B-4D05-B3CD-9ECF672D79CF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added release time for 9355B
</commit_message>
<xml_diff>
--- a/data/prepped/tag_release/lemhi_winter_telemetry_tag_info.xlsx
+++ b/data/prepped/tag_release/lemhi_winter_telemetry_tag_info.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\telemetyr\data\prepped\tag_release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B42266-37DA-41C8-A715-AEF68E968ACC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CB8B45-6D53-424B-BEE7-CDBC7C34B77E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="release_info" sheetId="1" r:id="rId1"/>
     <sheet name="batch_info" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">release_info!$A$1:$M$777</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7107" uniqueCount="1556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7106" uniqueCount="1556">
   <si>
     <t>season</t>
   </si>
@@ -5106,10 +5109,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M777"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A438" workbookViewId="0">
+      <selection activeCell="N425" sqref="N425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
@@ -8778,7 +8782,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>1</v>
       </c>
@@ -8819,7 +8823,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>1</v>
       </c>
@@ -8860,7 +8864,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>1</v>
       </c>
@@ -8901,7 +8905,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>1</v>
       </c>
@@ -8942,7 +8946,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>1</v>
       </c>
@@ -8983,7 +8987,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>1</v>
       </c>
@@ -9024,7 +9028,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>1</v>
       </c>
@@ -9065,7 +9069,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>1</v>
       </c>
@@ -9106,7 +9110,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>1</v>
       </c>
@@ -9147,7 +9151,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>1</v>
       </c>
@@ -9188,7 +9192,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>1</v>
       </c>
@@ -9229,7 +9233,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>1</v>
       </c>
@@ -9270,7 +9274,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>1</v>
       </c>
@@ -9311,7 +9315,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>1</v>
       </c>
@@ -9352,7 +9356,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>1</v>
       </c>
@@ -9393,7 +9397,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>1</v>
       </c>
@@ -9434,7 +9438,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>1</v>
       </c>
@@ -9475,7 +9479,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>1</v>
       </c>
@@ -9516,7 +9520,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>1</v>
       </c>
@@ -9557,7 +9561,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>1</v>
       </c>
@@ -9598,7 +9602,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>1</v>
       </c>
@@ -9639,7 +9643,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>1</v>
       </c>
@@ -9721,7 +9725,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>283</v>
       </c>
@@ -10541,7 +10545,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>283</v>
       </c>
@@ -10992,7 +10996,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>283</v>
       </c>
@@ -11812,7 +11816,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>283</v>
       </c>
@@ -12263,7 +12267,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>283</v>
       </c>
@@ -12509,7 +12513,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>283</v>
       </c>
@@ -13329,7 +13333,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>283</v>
       </c>
@@ -13534,7 +13538,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
         <v>283</v>
       </c>
@@ -14108,7 +14112,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
         <v>283</v>
       </c>
@@ -14231,7 +14235,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
         <v>283</v>
       </c>
@@ -14395,7 +14399,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
         <v>283</v>
       </c>
@@ -14477,7 +14481,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
         <v>283</v>
       </c>
@@ -14559,7 +14563,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
         <v>283</v>
       </c>
@@ -14641,7 +14645,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
         <v>283</v>
       </c>
@@ -14723,7 +14727,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
         <v>283</v>
       </c>
@@ -14805,7 +14809,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
         <v>283</v>
       </c>
@@ -14887,7 +14891,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
         <v>283</v>
       </c>
@@ -14969,7 +14973,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
         <v>283</v>
       </c>
@@ -15051,7 +15055,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
         <v>283</v>
       </c>
@@ -15133,7 +15137,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
         <v>283</v>
       </c>
@@ -15297,7 +15301,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
         <v>283</v>
       </c>
@@ -15953,7 +15957,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" s="2" t="s">
         <v>283</v>
       </c>
@@ -16691,7 +16695,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" s="2" t="s">
         <v>283</v>
       </c>
@@ -16855,7 +16859,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" s="2" t="s">
         <v>283</v>
       </c>
@@ -17142,7 +17146,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" s="2" t="s">
         <v>283</v>
       </c>
@@ -17470,7 +17474,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" s="2" t="s">
         <v>283</v>
       </c>
@@ -17552,7 +17556,7 @@
         <v>1547</v>
       </c>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" s="2" t="s">
         <v>283</v>
       </c>
@@ -17921,7 +17925,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" s="2" t="s">
         <v>283</v>
       </c>
@@ -17962,7 +17966,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" s="2" t="s">
         <v>283</v>
       </c>
@@ -18495,7 +18499,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327" s="2" t="s">
         <v>283</v>
       </c>
@@ -19192,7 +19196,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344" s="2" t="s">
         <v>283</v>
       </c>
@@ -19602,7 +19606,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A354" s="2" t="s">
         <v>283</v>
       </c>
@@ -20217,7 +20221,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369" s="2" t="s">
         <v>283</v>
       </c>
@@ -20422,7 +20426,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374" s="2" t="s">
         <v>283</v>
       </c>
@@ -20832,7 +20836,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A384" s="2" t="s">
         <v>283</v>
       </c>
@@ -21488,7 +21492,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="400" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A400" s="2" t="s">
         <v>283</v>
       </c>
@@ -21980,7 +21984,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="412" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A412" s="2" t="s">
         <v>283</v>
       </c>
@@ -22226,7 +22230,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="418" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A418" s="2" t="s">
         <v>283</v>
       </c>
@@ -23121,14 +23125,14 @@
       <c r="K439" s="3">
         <v>43395.247743055559</v>
       </c>
-      <c r="L439" s="8" t="s">
-        <v>115</v>
+      <c r="L439" s="8">
+        <v>43404.697916666664</v>
       </c>
       <c r="M439" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="440" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A440" s="2" t="s">
         <v>283</v>
       </c>
@@ -23374,7 +23378,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="446" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A446" s="2" t="s">
         <v>283</v>
       </c>
@@ -23456,7 +23460,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="448" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A448" s="2" t="s">
         <v>283</v>
       </c>
@@ -23772,7 +23776,7 @@
         <v>43760.791666666664</v>
       </c>
     </row>
-    <row r="456" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A456" s="2" t="s">
         <v>926</v>
       </c>
@@ -23810,7 +23814,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="457" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A457" s="2" t="s">
         <v>926</v>
       </c>
@@ -23889,7 +23893,7 @@
         <v>1543</v>
       </c>
     </row>
-    <row r="459" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A459" s="2" t="s">
         <v>926</v>
       </c>
@@ -23927,7 +23931,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="460" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A460" s="2" t="s">
         <v>926</v>
       </c>
@@ -23965,7 +23969,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="461" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A461" s="2" t="s">
         <v>926</v>
       </c>
@@ -24003,7 +24007,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="462" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A462" s="2" t="s">
         <v>926</v>
       </c>
@@ -24041,7 +24045,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="463" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A463" s="2" t="s">
         <v>926</v>
       </c>
@@ -26591,7 +26595,7 @@
         <v>43760.819444444445</v>
       </c>
     </row>
-    <row r="530" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A530" s="2" t="s">
         <v>926</v>
       </c>
@@ -27503,7 +27507,7 @@
         <v>43761.770833333336</v>
       </c>
     </row>
-    <row r="554" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="554" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A554" s="2" t="s">
         <v>926</v>
       </c>
@@ -28073,7 +28077,7 @@
         <v>43761.791666666664</v>
       </c>
     </row>
-    <row r="569" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A569" s="2" t="s">
         <v>926</v>
       </c>
@@ -28111,7 +28115,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="570" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="570" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A570" s="2" t="s">
         <v>926</v>
       </c>
@@ -28149,7 +28153,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="571" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A571" s="2" t="s">
         <v>926</v>
       </c>
@@ -28187,7 +28191,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="572" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A572" s="2" t="s">
         <v>926</v>
       </c>
@@ -28225,7 +28229,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="573" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A573" s="2" t="s">
         <v>926</v>
       </c>
@@ -28606,7 +28610,7 @@
         <v>43761.791666666664</v>
       </c>
     </row>
-    <row r="583" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="583" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A583" s="2" t="s">
         <v>926</v>
       </c>
@@ -28644,7 +28648,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="584" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="584" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A584" s="2" t="s">
         <v>926</v>
       </c>
@@ -28682,7 +28686,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="585" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="585" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A585" s="2" t="s">
         <v>926</v>
       </c>
@@ -28720,7 +28724,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="586" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="586" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A586" s="2" t="s">
         <v>926</v>
       </c>
@@ -28758,7 +28762,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="587" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A587" s="2" t="s">
         <v>926</v>
       </c>
@@ -28796,7 +28800,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="588" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A588" s="2" t="s">
         <v>926</v>
       </c>
@@ -28834,7 +28838,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="589" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A589" s="2" t="s">
         <v>926</v>
       </c>
@@ -28872,7 +28876,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="590" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="590" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A590" s="2" t="s">
         <v>926</v>
       </c>
@@ -28910,7 +28914,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="591" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="591" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A591" s="2" t="s">
         <v>926</v>
       </c>
@@ -28948,7 +28952,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="592" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="592" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A592" s="2" t="s">
         <v>926</v>
       </c>
@@ -29024,7 +29028,7 @@
         <v>43766.885416666664</v>
       </c>
     </row>
-    <row r="594" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="594" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A594" s="2" t="s">
         <v>926</v>
       </c>
@@ -29062,7 +29066,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="595" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A595" s="2" t="s">
         <v>926</v>
       </c>
@@ -29483,7 +29487,7 @@
         <v>43762.8125</v>
       </c>
     </row>
-    <row r="606" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A606" s="2" t="s">
         <v>926</v>
       </c>
@@ -30670,7 +30674,7 @@
         <v>43762.8125</v>
       </c>
     </row>
-    <row r="637" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="637" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A637" s="2" t="s">
         <v>926</v>
       </c>
@@ -30708,7 +30712,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="638" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="638" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A638" s="2" t="s">
         <v>926</v>
       </c>
@@ -30746,7 +30750,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="639" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="639" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A639" s="2" t="s">
         <v>926</v>
       </c>
@@ -33284,7 +33288,7 @@
         <v>43763.819444444445</v>
       </c>
     </row>
-    <row r="705" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="705" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A705" s="2" t="s">
         <v>926</v>
       </c>
@@ -34120,7 +34124,7 @@
         <v>43766.885416666664</v>
       </c>
     </row>
-    <row r="727" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="727" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A727" s="2" t="s">
         <v>926</v>
       </c>
@@ -35377,7 +35381,7 @@
         <v>43766.885416666664</v>
       </c>
     </row>
-    <row r="760" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="760" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A760" s="2" t="s">
         <v>926</v>
       </c>
@@ -35567,7 +35571,7 @@
         <v>43766.885416666664</v>
       </c>
     </row>
-    <row r="765" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="765" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A765" s="2" t="s">
         <v>926</v>
       </c>
@@ -35605,7 +35609,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="766" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="766" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A766" s="2" t="s">
         <v>926</v>
       </c>
@@ -35681,7 +35685,7 @@
         <v>43766.885416666664</v>
       </c>
     </row>
-    <row r="768" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="768" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A768" s="2" t="s">
         <v>926</v>
       </c>
@@ -35719,7 +35723,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="769" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="769" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A769" s="2" t="s">
         <v>926</v>
       </c>
@@ -35757,7 +35761,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="770" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="770" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A770" s="2" t="s">
         <v>926</v>
       </c>
@@ -35795,7 +35799,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="771" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="771" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A771" s="2" t="s">
         <v>926</v>
       </c>
@@ -35833,7 +35837,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="772" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="772" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A772" s="2" t="s">
         <v>926</v>
       </c>
@@ -35871,7 +35875,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="773" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="773" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A773" s="2" t="s">
         <v>926</v>
       </c>
@@ -35909,7 +35913,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="774" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="774" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A774" s="2" t="s">
         <v>926</v>
       </c>
@@ -35947,7 +35951,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="775" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="775" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A775" s="2" t="s">
         <v>926</v>
       </c>
@@ -36024,7 +36028,7 @@
       </c>
       <c r="M776" s="15"/>
     </row>
-    <row r="777" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="777" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A777" s="2" t="s">
         <v>926</v>
       </c>
@@ -36066,6 +36070,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M777" xr:uid="{D2A3B656-54CA-4D9D-90AF-20EAD761525A}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="fish"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36075,7 +36086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849A2B6F-9B4B-4D05-B3CD-9ECF672D79CF}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>